<commit_message>
Add enemies to all the rooms.
</commit_message>
<xml_diff>
--- a/Dantong Xue_Sprint0/Game1/Game1/Maps/Room/18.xlsx
+++ b/Dantong Xue_Sprint0/Game1/Game1/Maps/Room/18.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repo\CSE-3902\Dantong Xue_Sprint0\Game1\Game1\Maps\Room\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lianz\OneDrive\桌面\CSE-3902\Dantong Xue_Sprint0\Game1\Game1\Maps\Room\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B339CC-406D-4B23-B0E9-0717BB263F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4B9C4B-D9AF-476E-8F97-BE31BF155DFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1344" yWindow="1656" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="9">
   <si>
     <t>block</t>
     <phoneticPr fontId="19" type="noConversion"/>
@@ -34,20 +34,20 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>openDoorLeft</t>
+    <t>wallBack</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
+    <t>openDoorLeft</t>
+  </si>
+  <si>
     <t>wallRight</t>
-    <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
     <t>wallFront</t>
-    <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>wallBack</t>
-    <phoneticPr fontId="19" type="noConversion"/>
+    <t>block</t>
   </si>
   <si>
     <t>floatBlock</t>
@@ -57,11 +57,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -69,7 +69,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -77,7 +77,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="等线 Light"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -86,7 +86,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -95,7 +95,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -104,7 +104,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -112,7 +112,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -120,7 +120,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -128,7 +128,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -136,7 +136,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -145,7 +145,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -154,7 +154,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -162,7 +162,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -171,7 +171,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -179,7 +179,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -188,7 +188,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -197,7 +197,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -205,7 +205,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -218,7 +218,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -780,6 +780,63 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -807,107 +864,50 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -923,7 +923,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1222,53 +1222,53 @@
   <dimension ref="A1:AX30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="U9" activeCellId="1" sqref="I9:L14 U9:X14"/>
+      <selection activeCell="U15" sqref="U15:V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="32" width="2.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:50" ht="15" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="11" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="13"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="5"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
@@ -1288,39 +1288,39 @@
       <c r="AW1" s="1"/>
       <c r="AX1" s="1"/>
     </row>
-    <row r="2" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="16"/>
+    <row r="2" spans="1:50" ht="15" customHeight="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="8"/>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
@@ -1340,39 +1340,39 @@
       <c r="AW2" s="1"/>
       <c r="AX2" s="1"/>
     </row>
-    <row r="3" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="16"/>
+    <row r="3" spans="1:50" ht="15" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="8"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
@@ -1392,39 +1392,39 @@
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
     </row>
-    <row r="4" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="18"/>
-      <c r="Z4" s="18"/>
-      <c r="AA4" s="18"/>
-      <c r="AB4" s="18"/>
-      <c r="AC4" s="18"/>
-      <c r="AD4" s="18"/>
-      <c r="AE4" s="18"/>
-      <c r="AF4" s="19"/>
+    <row r="4" spans="1:50" ht="15" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="11"/>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
@@ -1444,67 +1444,67 @@
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
     </row>
-    <row r="5" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:50" ht="15" customHeight="1">
+      <c r="A5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="29"/>
-      <c r="AC5" s="2" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="4"/>
+      <c r="AD5" s="22"/>
+      <c r="AE5" s="22"/>
+      <c r="AF5" s="23"/>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
@@ -1524,39 +1524,39 @@
       <c r="AW5" s="1"/>
       <c r="AX5" s="1"/>
     </row>
-    <row r="6" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="29"/>
-      <c r="Z6" s="29"/>
-      <c r="AA6" s="29"/>
-      <c r="AB6" s="29"/>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="6"/>
-      <c r="AE6" s="6"/>
-      <c r="AF6" s="7"/>
+    <row r="6" spans="1:50" ht="15" customHeight="1">
+      <c r="A6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="24"/>
+      <c r="AD6" s="25"/>
+      <c r="AE6" s="25"/>
+      <c r="AF6" s="26"/>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
@@ -1576,63 +1576,63 @@
       <c r="AW6" s="1"/>
       <c r="AX6" s="1"/>
     </row>
-    <row r="7" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="T7" s="29"/>
-      <c r="U7" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="29"/>
-      <c r="AA7" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="29"/>
-      <c r="AC7" s="5"/>
-      <c r="AD7" s="6"/>
-      <c r="AE7" s="6"/>
-      <c r="AF7" s="7"/>
+    <row r="7" spans="1:50" ht="15" customHeight="1">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="24"/>
+      <c r="AD7" s="25"/>
+      <c r="AE7" s="25"/>
+      <c r="AF7" s="26"/>
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
@@ -1652,39 +1652,39 @@
       <c r="AW7" s="1"/>
       <c r="AX7" s="1"/>
     </row>
-    <row r="8" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="29"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="29"/>
-      <c r="X8" s="29"/>
-      <c r="Y8" s="29"/>
-      <c r="Z8" s="29"/>
-      <c r="AA8" s="29"/>
-      <c r="AB8" s="29"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="6"/>
-      <c r="AE8" s="6"/>
-      <c r="AF8" s="7"/>
+    <row r="8" spans="1:50" ht="15" customHeight="1">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="25"/>
+      <c r="AE8" s="25"/>
+      <c r="AF8" s="26"/>
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
@@ -1704,63 +1704,63 @@
       <c r="AW8" s="1"/>
       <c r="AX8" s="1"/>
     </row>
-    <row r="9" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29" t="s">
+    <row r="9" spans="1:50" ht="15" customHeight="1">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29" t="s">
+      <c r="N9" s="2"/>
+      <c r="O9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="X9" s="29"/>
-      <c r="Y9" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="29"/>
-      <c r="AA9" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="29"/>
-      <c r="AC9" s="8"/>
-      <c r="AD9" s="9"/>
-      <c r="AE9" s="9"/>
-      <c r="AF9" s="10"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="27"/>
+      <c r="AD9" s="28"/>
+      <c r="AE9" s="28"/>
+      <c r="AF9" s="29"/>
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
@@ -1780,43 +1780,43 @@
       <c r="AW9" s="1"/>
       <c r="AX9" s="1"/>
     </row>
-    <row r="10" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
-      <c r="Y10" s="29"/>
-      <c r="Z10" s="29"/>
-      <c r="AA10" s="29"/>
-      <c r="AB10" s="29"/>
-      <c r="AC10" s="20" t="s">
+    <row r="10" spans="1:50" ht="15" customHeight="1">
+      <c r="A10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AD10" s="21"/>
-      <c r="AE10" s="21"/>
-      <c r="AF10" s="22"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="14"/>
       <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
@@ -1836,63 +1836,63 @@
       <c r="AW10" s="1"/>
       <c r="AX10" s="1"/>
     </row>
-    <row r="11" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29" t="s">
+    <row r="11" spans="1:50" ht="15" customHeight="1">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29" t="s">
+      <c r="N11" s="2"/>
+      <c r="O11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="R11" s="29"/>
-      <c r="S11" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="T11" s="29"/>
-      <c r="U11" s="29" t="s">
+      <c r="T11" s="2"/>
+      <c r="U11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="V11" s="29"/>
-      <c r="W11" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="X11" s="29"/>
-      <c r="Y11" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="29"/>
-      <c r="AA11" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="29"/>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="24"/>
-      <c r="AE11" s="24"/>
-      <c r="AF11" s="25"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="15"/>
+      <c r="AD11" s="16"/>
+      <c r="AE11" s="16"/>
+      <c r="AF11" s="17"/>
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
@@ -1912,39 +1912,39 @@
       <c r="AW11" s="1"/>
       <c r="AX11" s="1"/>
     </row>
-    <row r="12" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29"/>
-      <c r="X12" s="29"/>
-      <c r="Y12" s="29"/>
-      <c r="Z12" s="29"/>
-      <c r="AA12" s="29"/>
-      <c r="AB12" s="29"/>
-      <c r="AC12" s="23"/>
-      <c r="AD12" s="24"/>
-      <c r="AE12" s="24"/>
-      <c r="AF12" s="25"/>
+    <row r="12" spans="1:50">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="16"/>
+      <c r="AE12" s="16"/>
+      <c r="AF12" s="17"/>
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
@@ -1964,63 +1964,63 @@
       <c r="AW12" s="1"/>
       <c r="AX12" s="1"/>
     </row>
-    <row r="13" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29" t="s">
+    <row r="13" spans="1:50">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="R13" s="29"/>
-      <c r="S13" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="T13" s="29"/>
-      <c r="U13" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="V13" s="29"/>
-      <c r="W13" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="X13" s="29"/>
-      <c r="Y13" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="29"/>
-      <c r="AA13" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="29"/>
-      <c r="AC13" s="26"/>
-      <c r="AD13" s="27"/>
-      <c r="AE13" s="27"/>
-      <c r="AF13" s="28"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="18"/>
+      <c r="AD13" s="19"/>
+      <c r="AE13" s="19"/>
+      <c r="AF13" s="20"/>
       <c r="AG13" s="1"/>
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
@@ -2040,43 +2040,43 @@
       <c r="AW13" s="1"/>
       <c r="AX13" s="1"/>
     </row>
-    <row r="14" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:50">
+      <c r="A14" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
-      <c r="S14" s="29"/>
-      <c r="T14" s="29"/>
-      <c r="U14" s="29"/>
-      <c r="V14" s="29"/>
-      <c r="W14" s="29"/>
-      <c r="X14" s="29"/>
-      <c r="Y14" s="29"/>
-      <c r="Z14" s="29"/>
-      <c r="AA14" s="29"/>
-      <c r="AB14" s="29"/>
-      <c r="AC14" s="2" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="AD14" s="3"/>
-      <c r="AE14" s="3"/>
-      <c r="AF14" s="4"/>
+      <c r="AD14" s="22"/>
+      <c r="AE14" s="22"/>
+      <c r="AF14" s="23"/>
       <c r="AG14" s="1"/>
       <c r="AH14" s="1"/>
       <c r="AI14" s="1"/>
@@ -2096,63 +2096,63 @@
       <c r="AW14" s="1"/>
       <c r="AX14" s="1"/>
     </row>
-    <row r="15" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="R15" s="29"/>
-      <c r="S15" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="T15" s="29"/>
-      <c r="U15" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="V15" s="29"/>
-      <c r="W15" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="X15" s="29"/>
-      <c r="Y15" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="29"/>
-      <c r="AA15" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="29"/>
-      <c r="AC15" s="5"/>
-      <c r="AD15" s="6"/>
-      <c r="AE15" s="6"/>
-      <c r="AF15" s="7"/>
+    <row r="15" spans="1:50">
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="24"/>
+      <c r="AD15" s="25"/>
+      <c r="AE15" s="25"/>
+      <c r="AF15" s="26"/>
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
@@ -2172,39 +2172,39 @@
       <c r="AW15" s="1"/>
       <c r="AX15" s="1"/>
     </row>
-    <row r="16" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
-      <c r="S16" s="29"/>
-      <c r="T16" s="29"/>
-      <c r="U16" s="29"/>
-      <c r="V16" s="29"/>
-      <c r="W16" s="29"/>
-      <c r="X16" s="29"/>
-      <c r="Y16" s="29"/>
-      <c r="Z16" s="29"/>
-      <c r="AA16" s="29"/>
-      <c r="AB16" s="29"/>
-      <c r="AC16" s="5"/>
-      <c r="AD16" s="6"/>
-      <c r="AE16" s="6"/>
-      <c r="AF16" s="7"/>
+    <row r="16" spans="1:50">
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="24"/>
+      <c r="AD16" s="25"/>
+      <c r="AE16" s="25"/>
+      <c r="AF16" s="26"/>
       <c r="AG16" s="1"/>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
@@ -2224,63 +2224,63 @@
       <c r="AW16" s="1"/>
       <c r="AX16" s="1"/>
     </row>
-    <row r="17" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="R17" s="29"/>
-      <c r="S17" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="T17" s="29"/>
-      <c r="U17" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="V17" s="29"/>
-      <c r="W17" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="X17" s="29"/>
-      <c r="Y17" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="29"/>
-      <c r="AA17" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="29"/>
-      <c r="AC17" s="5"/>
-      <c r="AD17" s="6"/>
-      <c r="AE17" s="6"/>
-      <c r="AF17" s="7"/>
+    <row r="17" spans="1:50">
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="24"/>
+      <c r="AD17" s="25"/>
+      <c r="AE17" s="25"/>
+      <c r="AF17" s="26"/>
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
@@ -2300,39 +2300,39 @@
       <c r="AW17" s="1"/>
       <c r="AX17" s="1"/>
     </row>
-    <row r="18" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="29"/>
-      <c r="T18" s="29"/>
-      <c r="U18" s="29"/>
-      <c r="V18" s="29"/>
-      <c r="W18" s="29"/>
-      <c r="X18" s="29"/>
-      <c r="Y18" s="29"/>
-      <c r="Z18" s="29"/>
-      <c r="AA18" s="29"/>
-      <c r="AB18" s="29"/>
-      <c r="AC18" s="8"/>
-      <c r="AD18" s="9"/>
-      <c r="AE18" s="9"/>
-      <c r="AF18" s="10"/>
+    <row r="18" spans="1:50">
+      <c r="A18" s="27"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="27"/>
+      <c r="AD18" s="28"/>
+      <c r="AE18" s="28"/>
+      <c r="AF18" s="29"/>
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
@@ -2352,45 +2352,45 @@
       <c r="AW18" s="1"/>
       <c r="AX18" s="1"/>
     </row>
-    <row r="19" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+    <row r="19" spans="1:50">
+      <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="11" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="T19" s="12"/>
-      <c r="U19" s="12"/>
-      <c r="V19" s="12"/>
-      <c r="W19" s="12"/>
-      <c r="X19" s="12"/>
-      <c r="Y19" s="12"/>
-      <c r="Z19" s="12"/>
-      <c r="AA19" s="12"/>
-      <c r="AB19" s="12"/>
-      <c r="AC19" s="12"/>
-      <c r="AD19" s="12"/>
-      <c r="AE19" s="12"/>
-      <c r="AF19" s="13"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="5"/>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
@@ -2410,39 +2410,39 @@
       <c r="AW19" s="1"/>
       <c r="AX19" s="1"/>
     </row>
-    <row r="20" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="15"/>
-      <c r="Z20" s="15"/>
-      <c r="AA20" s="15"/>
-      <c r="AB20" s="15"/>
-      <c r="AC20" s="15"/>
-      <c r="AD20" s="15"/>
-      <c r="AE20" s="15"/>
-      <c r="AF20" s="16"/>
+    <row r="20" spans="1:50">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="7"/>
+      <c r="AF20" s="8"/>
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
@@ -2462,39 +2462,39 @@
       <c r="AW20" s="1"/>
       <c r="AX20" s="1"/>
     </row>
-    <row r="21" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="15"/>
-      <c r="Z21" s="15"/>
-      <c r="AA21" s="15"/>
-      <c r="AB21" s="15"/>
-      <c r="AC21" s="15"/>
-      <c r="AD21" s="15"/>
-      <c r="AE21" s="15"/>
-      <c r="AF21" s="16"/>
+    <row r="21" spans="1:50">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7"/>
+      <c r="AC21" s="7"/>
+      <c r="AD21" s="7"/>
+      <c r="AE21" s="7"/>
+      <c r="AF21" s="8"/>
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
@@ -2514,39 +2514,39 @@
       <c r="AW21" s="1"/>
       <c r="AX21" s="1"/>
     </row>
-    <row r="22" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="28"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="18"/>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18"/>
-      <c r="W22" s="18"/>
-      <c r="X22" s="18"/>
-      <c r="Y22" s="18"/>
-      <c r="Z22" s="18"/>
-      <c r="AA22" s="18"/>
-      <c r="AB22" s="18"/>
-      <c r="AC22" s="18"/>
-      <c r="AD22" s="18"/>
-      <c r="AE22" s="18"/>
-      <c r="AF22" s="19"/>
+    <row r="22" spans="1:50">
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="10"/>
+      <c r="AD22" s="10"/>
+      <c r="AE22" s="10"/>
+      <c r="AF22" s="11"/>
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
@@ -2566,7 +2566,7 @@
       <c r="AW22" s="1"/>
       <c r="AX22" s="1"/>
     </row>
-    <row r="23" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:50">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2618,7 +2618,7 @@
       <c r="AW23" s="1"/>
       <c r="AX23" s="1"/>
     </row>
-    <row r="24" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2670,7 +2670,7 @@
       <c r="AW24" s="1"/>
       <c r="AX24" s="1"/>
     </row>
-    <row r="25" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2722,7 +2722,7 @@
       <c r="AW25" s="1"/>
       <c r="AX25" s="1"/>
     </row>
-    <row r="26" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2774,7 +2774,7 @@
       <c r="AW26" s="1"/>
       <c r="AX26" s="1"/>
     </row>
-    <row r="27" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2826,7 +2826,7 @@
       <c r="AW27" s="1"/>
       <c r="AX27" s="1"/>
     </row>
-    <row r="28" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2878,7 +2878,7 @@
       <c r="AW28" s="1"/>
       <c r="AX28" s="1"/>
     </row>
-    <row r="29" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:50">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2930,7 +2930,7 @@
       <c r="AW29" s="1"/>
       <c r="AX29" s="1"/>
     </row>
-    <row r="30" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:50">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2984,86 +2984,6 @@
     </row>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="AA5:AB6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="G5:H6"/>
-    <mergeCell ref="I5:J6"/>
-    <mergeCell ref="K5:L6"/>
-    <mergeCell ref="M5:N6"/>
-    <mergeCell ref="O5:P6"/>
-    <mergeCell ref="Q5:R6"/>
-    <mergeCell ref="S5:T6"/>
-    <mergeCell ref="U5:V6"/>
-    <mergeCell ref="W5:X6"/>
-    <mergeCell ref="Y5:Z6"/>
-    <mergeCell ref="AA7:AB8"/>
-    <mergeCell ref="E7:F8"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="I7:J8"/>
-    <mergeCell ref="K7:L8"/>
-    <mergeCell ref="M7:N8"/>
-    <mergeCell ref="O7:P8"/>
-    <mergeCell ref="Q7:R8"/>
-    <mergeCell ref="S7:T8"/>
-    <mergeCell ref="U7:V8"/>
-    <mergeCell ref="W7:X8"/>
-    <mergeCell ref="Y7:Z8"/>
-    <mergeCell ref="AA9:AB10"/>
-    <mergeCell ref="E9:F10"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="M9:N10"/>
-    <mergeCell ref="O9:P10"/>
-    <mergeCell ref="Q9:R10"/>
-    <mergeCell ref="S9:T10"/>
-    <mergeCell ref="U9:V10"/>
-    <mergeCell ref="W9:X10"/>
-    <mergeCell ref="Y9:Z10"/>
-    <mergeCell ref="AA11:AB12"/>
-    <mergeCell ref="E11:F12"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="I11:J12"/>
-    <mergeCell ref="K11:L12"/>
-    <mergeCell ref="M11:N12"/>
-    <mergeCell ref="O11:P12"/>
-    <mergeCell ref="Q11:R12"/>
-    <mergeCell ref="S11:T12"/>
-    <mergeCell ref="U11:V12"/>
-    <mergeCell ref="W11:X12"/>
-    <mergeCell ref="Y11:Z12"/>
-    <mergeCell ref="AA13:AB14"/>
-    <mergeCell ref="E13:F14"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="I13:J14"/>
-    <mergeCell ref="K13:L14"/>
-    <mergeCell ref="M13:N14"/>
-    <mergeCell ref="O13:P14"/>
-    <mergeCell ref="Q13:R14"/>
-    <mergeCell ref="S13:T14"/>
-    <mergeCell ref="U13:V14"/>
-    <mergeCell ref="W13:X14"/>
-    <mergeCell ref="Y13:Z14"/>
-    <mergeCell ref="AA15:AB16"/>
-    <mergeCell ref="E15:F16"/>
-    <mergeCell ref="G15:H16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="K15:L16"/>
-    <mergeCell ref="M15:N16"/>
-    <mergeCell ref="O15:P16"/>
-    <mergeCell ref="Q15:R16"/>
-    <mergeCell ref="S15:T16"/>
-    <mergeCell ref="U15:V16"/>
-    <mergeCell ref="W15:X16"/>
-    <mergeCell ref="Y15:Z16"/>
-    <mergeCell ref="S17:T18"/>
-    <mergeCell ref="A19:N22"/>
-    <mergeCell ref="S19:AF22"/>
-    <mergeCell ref="O19:R22"/>
-    <mergeCell ref="U17:V18"/>
-    <mergeCell ref="W17:X18"/>
-    <mergeCell ref="Y17:Z18"/>
-    <mergeCell ref="K17:L18"/>
     <mergeCell ref="A5:D9"/>
     <mergeCell ref="A1:N4"/>
     <mergeCell ref="S1:AF4"/>
@@ -3080,6 +3000,86 @@
     <mergeCell ref="M17:N18"/>
     <mergeCell ref="O17:P18"/>
     <mergeCell ref="Q17:R18"/>
+    <mergeCell ref="S17:T18"/>
+    <mergeCell ref="A19:N22"/>
+    <mergeCell ref="S19:AF22"/>
+    <mergeCell ref="O19:R22"/>
+    <mergeCell ref="U17:V18"/>
+    <mergeCell ref="W17:X18"/>
+    <mergeCell ref="Y17:Z18"/>
+    <mergeCell ref="K17:L18"/>
+    <mergeCell ref="AA15:AB16"/>
+    <mergeCell ref="E15:F16"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="K15:L16"/>
+    <mergeCell ref="M15:N16"/>
+    <mergeCell ref="O15:P16"/>
+    <mergeCell ref="Q15:R16"/>
+    <mergeCell ref="S15:T16"/>
+    <mergeCell ref="U15:V16"/>
+    <mergeCell ref="W15:X16"/>
+    <mergeCell ref="Y15:Z16"/>
+    <mergeCell ref="AA13:AB14"/>
+    <mergeCell ref="E13:F14"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="I13:J14"/>
+    <mergeCell ref="K13:L14"/>
+    <mergeCell ref="M13:N14"/>
+    <mergeCell ref="O13:P14"/>
+    <mergeCell ref="Q13:R14"/>
+    <mergeCell ref="S13:T14"/>
+    <mergeCell ref="U13:V14"/>
+    <mergeCell ref="W13:X14"/>
+    <mergeCell ref="Y13:Z14"/>
+    <mergeCell ref="AA11:AB12"/>
+    <mergeCell ref="E11:F12"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="I11:J12"/>
+    <mergeCell ref="K11:L12"/>
+    <mergeCell ref="M11:N12"/>
+    <mergeCell ref="O11:P12"/>
+    <mergeCell ref="Q11:R12"/>
+    <mergeCell ref="S11:T12"/>
+    <mergeCell ref="U11:V12"/>
+    <mergeCell ref="W11:X12"/>
+    <mergeCell ref="Y11:Z12"/>
+    <mergeCell ref="AA9:AB10"/>
+    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="M9:N10"/>
+    <mergeCell ref="O9:P10"/>
+    <mergeCell ref="Q9:R10"/>
+    <mergeCell ref="S9:T10"/>
+    <mergeCell ref="U9:V10"/>
+    <mergeCell ref="W9:X10"/>
+    <mergeCell ref="Y9:Z10"/>
+    <mergeCell ref="AA7:AB8"/>
+    <mergeCell ref="E7:F8"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="I7:J8"/>
+    <mergeCell ref="K7:L8"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="O7:P8"/>
+    <mergeCell ref="Q7:R8"/>
+    <mergeCell ref="S7:T8"/>
+    <mergeCell ref="U7:V8"/>
+    <mergeCell ref="W7:X8"/>
+    <mergeCell ref="Y7:Z8"/>
+    <mergeCell ref="AA5:AB6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="G5:H6"/>
+    <mergeCell ref="I5:J6"/>
+    <mergeCell ref="K5:L6"/>
+    <mergeCell ref="M5:N6"/>
+    <mergeCell ref="O5:P6"/>
+    <mergeCell ref="Q5:R6"/>
+    <mergeCell ref="S5:T6"/>
+    <mergeCell ref="U5:V6"/>
+    <mergeCell ref="W5:X6"/>
+    <mergeCell ref="Y5:Z6"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>